<commit_message>
Implemented successfully excel sheet for the data driven testing in Asset, assets types, Leave balance, Leave types, Project, JobTitles
</commit_message>
<xml_diff>
--- a/ExcelData/TC_DailyUpdates.xlsx
+++ b/ExcelData/TC_DailyUpdates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23370" windowHeight="10740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23370" windowHeight="12930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>dailyUpdateDate</t>
   </si>
@@ -59,15 +59,15 @@
   </si>
   <si>
     <t>time pass</t>
+  </si>
+  <si>
+    <t>17 August 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,12 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -426,7 +423,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,57 +432,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>45155</v>
-      </c>
-      <c r="B2" s="5">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
         <v>55</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4">
         <v>9</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="4">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">

</xml_diff>